<commit_message>
R script working again
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -30,9 +30,6 @@
     <t>categoryA</t>
   </si>
   <si>
-    <t>insects</t>
-  </si>
-  <si>
     <t>leftAttribute</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Flowers</t>
+  </si>
+  <si>
+    <t>Insects</t>
   </si>
 </sst>
 </file>
@@ -144,8 +144,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,7 +290,7 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -351,6 +353,7 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -413,6 +416,7 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -744,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -764,153 +768,153 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="180">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="135">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="120">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="120">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="120">
       <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="120">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
D1 calculation corrections to R script, block order correction to psychopy script
</commit_message>
<xml_diff>
--- a/instructions.xlsx
+++ b/instructions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
@@ -97,6 +97,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,7 +145,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,11 +273,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -289,8 +297,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="135">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +364,10 @@
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -417,6 +431,10 @@
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3 C3 D2 D2 E2 F2 F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -778,59 +796,59 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="180">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="135">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="120">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
@@ -838,19 +856,19 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="120">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
@@ -858,13 +876,13 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="120">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
@@ -878,19 +896,19 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="120">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
@@ -898,19 +916,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="120">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">

</xml_diff>